<commit_message>
Refactoring to get ready to add a second input format.
</commit_message>
<xml_diff>
--- a/packingSlipTemplate.xlsx
+++ b/packingSlipTemplate.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\auld\goDev\src\packingSlips\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\auld\godev\src\github.com\willauld\packingSlips\packingSlips\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="120" windowWidth="12975" windowHeight="8100"/>
+    <workbookView xWindow="5652" yWindow="120" windowWidth="12972" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="Packing slip" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Packing slip'!$A$1:$G$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Packing slip'!$B$1:$G$32</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
@@ -593,26 +593,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -642,7 +622,27 @@
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -752,7 +752,7 @@
         <xdr:cNvPr id="1038" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -887,23 +887,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -939,23 +922,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1137,91 +1103,91 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:D22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B1:G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.73046875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="4.86328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.73046875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.73046875" style="2" customWidth="1"/>
-    <col min="6" max="7" width="16.73046875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="1"/>
+    <col min="2" max="2" width="19.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="4.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="16.77734375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="G1" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E2" s="23"/>
-      <c r="F2" s="51">
+      <c r="F2" s="43">
         <f ca="1">TODAY()</f>
-        <v>42784</v>
-      </c>
-      <c r="G2" s="51"/>
-    </row>
-    <row r="3" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>42894</v>
+      </c>
+      <c r="G2" s="43"/>
+    </row>
+    <row r="3" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="25"/>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="2:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="45" t="s">
+    <row r="6" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="45"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
+    <row r="7" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
+    <row r="9" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
     </row>
-    <row r="11" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E11" s="13"/>
       <c r="F11" s="20"/>
     </row>
-    <row r="12" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>1</v>
       </c>
@@ -1237,7 +1203,7 @@
       </c>
       <c r="G12" s="19"/>
     </row>
-    <row r="13" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13"/>
       <c r="C13" s="33" t="s">
         <v>19</v>
@@ -1249,7 +1215,7 @@
       </c>
       <c r="G13" s="22"/>
     </row>
-    <row r="14" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13"/>
       <c r="C14" s="33" t="s">
         <v>20</v>
@@ -1261,7 +1227,7 @@
       </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="13"/>
       <c r="C15" s="33" t="s">
         <v>21</v>
@@ -1271,7 +1237,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
@@ -1280,7 +1246,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1289,15 +1255,15 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="46"/>
+      <c r="D18" s="62"/>
       <c r="E18" s="17" t="s">
         <v>10</v>
       </c>
@@ -1308,11 +1274,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="41"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="64"/>
       <c r="E19" s="37"/>
       <c r="F19" s="38"/>
       <c r="G19" s="31" t="str">
@@ -1320,11 +1286,11 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="42"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="58"/>
       <c r="E20" s="30"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32" t="str">
@@ -1332,11 +1298,11 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="41"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="29"/>
       <c r="F21" s="31"/>
       <c r="G21" s="31" t="str">
@@ -1344,11 +1310,11 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="42"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="58"/>
       <c r="E22" s="30"/>
       <c r="F22" s="32"/>
       <c r="G22" s="32" t="str">
@@ -1356,11 +1322,11 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="41"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="29"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31" t="str">
@@ -1368,11 +1334,11 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="42"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="64"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="59"/>
       <c r="E24" s="30"/>
       <c r="F24" s="32"/>
       <c r="G24" s="32" t="str">
@@ -1380,13 +1346,13 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="27"/>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="61"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="29"/>
       <c r="F25" s="31"/>
       <c r="G25" s="31" t="str">
@@ -1394,7 +1360,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="28"/>
       <c r="C26" s="36"/>
@@ -1406,46 +1372,46 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="59" t="s">
+      <c r="E27" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="59"/>
+      <c r="F27" s="51"/>
       <c r="G27" s="40">
         <f>SUM(G19:G26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
-      <c r="E28" s="59" t="s">
+      <c r="E28" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="59"/>
+      <c r="F28" s="51"/>
       <c r="G28" s="40"/>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
-      <c r="E29" s="59" t="s">
+      <c r="E29" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="59"/>
+      <c r="F29" s="51"/>
       <c r="G29" s="40">
         <f>SUM(G27:G28)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -1454,27 +1420,27 @@
       <c r="F30" s="15"/>
       <c r="G30" s="39"/>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
-      <c r="B31" s="52" t="s">
+      <c r="B31" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="53"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="55"/>
-    </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="45"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="47"/>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="58"/>
-    </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="50"/>
+    </row>
+    <row r="33" spans="1:7" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -1483,7 +1449,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" ht="11.25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="3" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1493,6 +1459,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B31:G32"/>
     <mergeCell ref="E28:F28"/>
@@ -1504,12 +1476,6 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>